<commit_message>
added new abx, added new ruling to ESBL per site, Transformed MIC Columns
</commit_message>
<xml_diff>
--- a/whonet/static/whonet_xl/whonet_codes_location_2020.xlsx
+++ b/whonet/static/whonet_xl/whonet_codes_location_2020.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT\dmu_sys\whonet\static\whonet_xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="715" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" tabRatio="715" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="bgh" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15347" uniqueCount="1838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15352" uniqueCount="1838">
   <si>
     <t>ent</t>
   </si>
@@ -21359,15 +21359,19 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1311"/>
+  <dimension ref="A1:E1312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1277" workbookViewId="0">
-      <selection activeCell="E1311" sqref="E1311"/>
+    <sheetView tabSelected="1" topLeftCell="A1248" workbookViewId="0">
+      <selection activeCell="A1312" sqref="A1312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -41917,6 +41921,23 @@
         <v>6</v>
       </c>
       <c r="E1311" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1312" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1312" t="s">
+        <v>260</v>
+      </c>
+      <c r="C1312" t="s">
+        <v>1837</v>
+      </c>
+      <c r="D1312" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1312" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>